<commit_message>
Listo y funcional!!! trabajar con python 3.11.9
</commit_message>
<xml_diff>
--- a/Finanzas-Visuales-analisis-y-gestion-simple-para-microempresas-con-IA/uploads/Indicadores_Financieros_Basicos_Calculados_v3.xlsx
+++ b/Finanzas-Visuales-analisis-y-gestion-simple-para-microempresas-con-IA/uploads/Indicadores_Financieros_Basicos_Calculados_v3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Samsung\Proyecto\Proyecto_python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E2A2CBB-A4BC-466C-90D6-38090755D377}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B34A4B12-F5AF-4A47-B1D3-7959AD499627}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="10455" windowHeight="10905" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10140" yWindow="0" windowWidth="10455" windowHeight="10905" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instrucciones" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="92">
   <si>
     <t>INSTRUCCIONES PARA LLENAR LA PLANTILLA</t>
   </si>
@@ -247,13 +247,79 @@
   </si>
   <si>
     <t xml:space="preserve">Debe ser igual al total de activos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Análisis Vertical </t>
+  </si>
+  <si>
+    <t xml:space="preserve">item </t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pasivos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patrimonio </t>
+  </si>
+  <si>
+    <t>Total en %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Análisis Horizontal </t>
+  </si>
+  <si>
+    <t>Utilidad neta</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total de ingresos - total costos y gastos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interpretación </t>
+  </si>
+  <si>
+    <t>Las ventas crecieron un 21%, lo cual indica un aumento positivo en la demanda o en la eficiencia comercial. La empresa está generando más ingresos respecto al periodo anterior.</t>
+  </si>
+  <si>
+    <t>El incremento es aún mayor que el de las ventas, lo que puede reflejar diversificación de fuentes de ingreso (por ejemplo, rentas, servicios adicionales, inversiones o ingresos financieros). Esto fortalece la estructura de ingresos.</t>
+  </si>
+  <si>
+    <t>Crece al mismo ritmo que las ventas, lo que sugiere que los costos se mantienen controlados; la empresa mantiene su margen bruto estable, sin deterioro de eficiencia productiva.</t>
+  </si>
+  <si>
+    <t>Aumentan en menor proporción que las ventas, lo que es positivo. Indica mejor gestión administrativa y de control de gastos, o un mayor aprovechamiento de economías de escala</t>
+  </si>
+  <si>
+    <t>El crecimiento es ligeramente mayor que el de las ventas; esto puede deberse a mayor endeudamiento o tasas de interés más altas. Conviene vigilar este rubro para evitar que afecte la rentabilidad neta.</t>
+  </si>
+  <si>
+    <t>Aumentan casi en la misma proporción que la utilidad antes de impuestos, lo que es coherente con el crecimiento de las utilidades. Refleja un mayor volumen de operaciones y ganancias.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROA </t>
+  </si>
+  <si>
+    <t>ROE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Punto de Equilibrio </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Liquidez </t>
+  </si>
+  <si>
+    <t>Por cada quetzal de deuda a corto plazo, la empresa tiene Q2.125 disponibles en activos corrientes.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -274,8 +340,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -294,8 +367,14 @@
         <bgColor rgb="FFFFF2CC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -329,11 +408,172 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFBFBFBF"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFBFBFBF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFBFBFBF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFBFBFBF"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -348,11 +588,45 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -365,6 +639,1941 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-GT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>estado_resultados!$B$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>estado_resultados!$A$18:$A$23</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Ventas totales</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Otros ingresos</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Costo de ventas</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Gastos de operación</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Gastos financieros</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Impuestos</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>estado_resultados!$B$18:$B$23</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.20833333333333334</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.33333333333333331</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.20833333333333334</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.10714285714285714</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.22222222222222221</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-52D1-4EF3-BF82-A237B939520F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="1984852511"/>
+        <c:axId val="1984850111"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1984852511"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-GT"/>
+                  <a:t>Concepto</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-GT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-GT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1984850111"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1984850111"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-GT"/>
+                  <a:t>%Variación</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-GT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-GT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1984852511"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-GT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-GT"/>
+              <a:t>Análisis Vertical</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-GT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>balance_general!$A$23:$A$26</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Efectivo y bancos</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Cuentas por cobrar</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Inventarios</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Activos fijos</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>balance_general!$B$23:$B$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>14.117647058823529</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21.176470588235293</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23.52941176470588</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41.17647058823529</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F814-47C3-9929-4861FCCDE24C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-GT"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-GT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>499560</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>75197</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>539665</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>148891</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D8EA29EE-CB80-2F9C-50CE-25514A2FC120}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>201083</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>184149</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>650874</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C089D818-2CA6-85CA-7294-59F8442D06C7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>457199</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1" descr="Imagen generada">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F95A8D55-AFC9-6C27-1D7E-1590EDCB8FDC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3009900" y="1152525"/>
+          <a:ext cx="2581274" cy="2581274"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -746,7 +2955,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6B25375-28B8-4B21-A1FE-295D8E8D628D}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -803,10 +3012,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF25E03F-B4CB-4636-AB7F-ADD3CFFF2635}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView zoomScale="76" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -868,86 +3077,243 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
+      <c r="A5" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="15">
+        <f>SUM(B3:B4)</f>
+        <v>1230000</v>
+      </c>
+      <c r="C5" s="15">
+        <f>SUM(C3:C4)</f>
+        <v>1490000</v>
+      </c>
       <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="3"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="4">
-        <v>720000</v>
-      </c>
-      <c r="C7" s="4">
-        <v>870000</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" s="4">
-        <v>280000</v>
-      </c>
-      <c r="C8" s="4">
-        <v>310000</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>32</v>
-      </c>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="5"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B9" s="4">
-        <v>18000</v>
+        <v>720000</v>
       </c>
       <c r="C9" s="4">
-        <v>22000</v>
+        <v>870000</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="4">
+        <v>280000</v>
+      </c>
+      <c r="C10" s="4">
+        <v>310000</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="4">
+        <v>18000</v>
+      </c>
+      <c r="C11" s="4">
+        <v>22000</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B12" s="4">
         <v>25000</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C12" s="4">
         <v>30000</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D12" s="3" t="s">
         <v>36</v>
       </c>
     </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="B13">
+        <f>SUM(B9:B12)</f>
+        <v>1043000</v>
+      </c>
+      <c r="C13">
+        <f>SUM(C9:C12)</f>
+        <v>1232000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14">
+        <f>B5-B13</f>
+        <v>187000</v>
+      </c>
+      <c r="C14">
+        <f>C5-C13</f>
+        <v>258000</v>
+      </c>
+      <c r="D14" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="B17" s="29"/>
+      <c r="C17" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="21">
+        <f>(C3-B3)/B3</f>
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="19">
+        <f>(C4-B4)/B4</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="19">
+        <f>(C9-B9)/B9</f>
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="19">
+        <f>(C10-B10)/B10</f>
+        <v>0.10714285714285714</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="19">
+        <f>(C11-B11)/B11</f>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="19">
+        <f>(C12-B12)/B12</f>
+        <v>0.2</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="14"/>
+    </row>
+    <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="B26" s="23">
+        <f>(B14/850000)</f>
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="B27" s="25">
+        <f>(187000/450000)</f>
+        <v>0.41555555555555557</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A17:B17"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24A283E7-BD79-4230-BB73-016053394E93}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView zoomScale="75" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1040,11 +3406,11 @@
       <c r="A7" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="3">
         <f>SUM(B3:B6)</f>
         <v>850000</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="3">
         <f>SUM(C3:C6)</f>
         <v>960000</v>
       </c>
@@ -1054,8 +3420,8 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
       <c r="D8" s="3"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1098,11 +3464,11 @@
       <c r="A12" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12" s="3">
         <f>SUM(B10:B11)</f>
         <v>400000</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="3">
         <f>SUM(C10:C11)</f>
         <v>410000</v>
       </c>
@@ -1110,8 +3476,8 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
       <c r="D13" s="3"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1151,7 +3517,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="8" t="s">
         <v>67</v>
       </c>
       <c r="B17">
@@ -1179,17 +3545,117 @@
         <v>69</v>
       </c>
     </row>
+    <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21" s="31"/>
+      <c r="C21" s="32"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" t="s">
+        <v>72</v>
+      </c>
+      <c r="C22" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23">
+        <f>(B3/B7)*100</f>
+        <v>14.117647058823529</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24">
+        <f>(B4/B7)*100</f>
+        <v>21.176470588235293</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25">
+        <f>(B5/B7)*100</f>
+        <v>23.52941176470588</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" s="10">
+        <f>(B6/B7)*100</f>
+        <v>41.17647058823529</v>
+      </c>
+      <c r="C26" s="11">
+        <f>SUM(B23:B26)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B27">
+        <f>(B12/B19)*100</f>
+        <v>47.058823529411761</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="B28" s="11">
+        <f>(B17/B19)*100</f>
+        <v>52.941176470588239</v>
+      </c>
+      <c r="C28" s="11">
+        <f>SUM(B27:B28)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="B32" s="27">
+        <f>B7/B12</f>
+        <v>2.125</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>91</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A21:C21"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E94A205-D345-4132-9042-8C82C7028E1A}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1253,7 +3719,18 @@
         <v>63</v>
       </c>
     </row>
+    <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="B9" s="27">
+        <f>B4/(B2-B3)</f>
+        <v>1888.8888888888889</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>